<commit_message>
In this is commit, I was added navigation and I make then that user authorization was without phone number
</commit_message>
<xml_diff>
--- a/tgbot/data/locales/local.xlsx
+++ b/tgbot/data/locales/local.xlsx
@@ -15,19 +15,157 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Ключевой текст</t>
   </si>
   <si>
-    <t>Қазақша</t>
+    <t>UZB</t>
+  </si>
+  <si>
+    <t>Введите ваше имя</t>
+  </si>
+  <si>
+    <t>Выберите язык</t>
+  </si>
+  <si>
+    <t>Вы успешно авторизовались.</t>
+  </si>
+  <si>
+    <t>Ваша корзина</t>
+  </si>
+  <si>
+    <t>В корзине пусто</t>
+  </si>
+  <si>
+    <t>Прикрепить чек</t>
+  </si>
+  <si>
+    <t>Назад на главную</t>
+  </si>
+  <si>
+    <t>Скиньте скриншот чека или pdf</t>
+  </si>
+  <si>
+    <t>Вы отправили не правильный файл, пожалуйста Скиньте скриншот чека или файл в формате pdf</t>
+  </si>
+  <si>
+    <t>Ваш файл не в формате pdf. Cкиньте скриншот чека или файл в формате pdf</t>
+  </si>
+  <si>
+    <t>Спасибо за покупку, скоро администратор примет вашу заявку</t>
+  </si>
+  <si>
+    <t>Выберите товар</t>
+  </si>
+  <si>
+    <t>Нет товаров в наличи</t>
+  </si>
+  <si>
+    <t>Поделитесь номером телефона для авторизации</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>Ваш заказ</t>
+  </si>
+  <si>
+    <t>Итого</t>
+  </si>
+  <si>
+    <t>Для оплаты перейдите по &lt;a href = "https://www.google.kz/?hl=ru"&gt;ссылке&lt;/a&gt; и оплатите</t>
+  </si>
+  <si>
+    <t>Чек оплаты прикрепить, нажав кнопку "Прикрепить чек" ниже (скриншот чека или pdf)</t>
+  </si>
+  <si>
+    <t>Поделиться телефоном</t>
+  </si>
+  <si>
+    <t>Каталог</t>
+  </si>
+  <si>
+    <t>Корзина</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+  </si>
+  <si>
+    <t>Контакты</t>
+  </si>
+  <si>
+    <t>Сменить язык</t>
+  </si>
+  <si>
+    <t>Назад</t>
+  </si>
+  <si>
+    <t>Купить</t>
+  </si>
+  <si>
+    <t>Очистить корзину</t>
+  </si>
+  <si>
+    <t>Новый заказ!</t>
+  </si>
+  <si>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>Мобильный телефон</t>
+  </si>
+  <si>
+    <t>Заказ</t>
+  </si>
+  <si>
+    <t>Вы сменили язык</t>
+  </si>
+  <si>
+    <t>Ederra Lab 01 Sulfate Free шампунь 600 мл</t>
+  </si>
+  <si>
+    <t>Ederra Lab 01 шампунь 600 мл</t>
+  </si>
+  <si>
+    <t>Ederra Lab 03 спрей-кондиционер 200 мл</t>
+  </si>
+  <si>
+    <t>Ederra Lab 02 Intense Moisture Mask маска 600 мл</t>
+  </si>
+  <si>
+    <t>Ederra Lab 01 Sulfate Free шампунь 300 мл</t>
+  </si>
+  <si>
+    <t>Ederra Lab 01 шампунь 300 мл</t>
+  </si>
+  <si>
+    <t>придание блеска, увлажнение, питание, укрепление, придание эластичности, восстановление, очищение, защита</t>
+  </si>
+  <si>
+    <t>увлажнение, питание, разглаживание, укрепление, придание эластичности, антистатический эффект, против секущихся концов, защита, восстановление</t>
+  </si>
+  <si>
+    <t>Содержит комплекс витаминов А, В, Е, F, D, высокую концентрацию активного ингредиента листьев чайного дерева и гидролизованный коллаген. Восстанавливает волосы на молекулярном уровне. Питает и укрепляет, увлажняет волосы и кожу головы, оказывает себорегулирующее воздействие. Придаёт волосам мягкость, эластичность, естественный блеск и упругость.</t>
+  </si>
+  <si>
+    <t>Специальная концентрированная формула изготовлена на натуральной основе листьев чайного дерева. Содержит комплекс витаминов А, В, E, F, D, коллаген и экстракт листьев алоэ Barbadensis.</t>
+  </si>
+  <si>
+    <t>Специальная концентрированная формула изготовлена на натуральной основе листьев чайного дерева. Эффективно и бережно очищает волосы и кожу головы, исключая их пересушивание.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -35,9 +173,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -64,7 +213,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -275,15 +424,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="92.5703125" customWidth="1"/>
+    <col min="1" max="1" width="102.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -291,12 +440,263 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A38" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A39" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A40" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A41" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A42" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A43" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A44" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A45" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A46" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A47" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A48" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A49" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A50" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A51" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
In this is commit, I was added FAQ and new button "coop" and updated dictionary from local
</commit_message>
<xml_diff>
--- a/tgbot/data/locales/local.xlsx
+++ b/tgbot/data/locales/local.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="125">
   <si>
     <t>Ключевой текст</t>
   </si>
@@ -159,6 +159,259 @@
   </si>
   <si>
     <t>Специальная концентрированная формула изготовлена на натуральной основе листьев чайного дерева. Эффективно и бережно очищает волосы и кожу головы, исключая их пересушивание.</t>
+  </si>
+  <si>
+    <t>Ismingizni kiriting</t>
+  </si>
+  <si>
+    <t>Tilni tanlang</t>
+  </si>
+  <si>
+    <t>Siz muvaffaqiyatli tizimga kirdingiz.</t>
+  </si>
+  <si>
+    <t>Sizning savatingiz</t>
+  </si>
+  <si>
+    <t>Arava bo‘sh</t>
+  </si>
+  <si>
+    <t>Chekni biriktiring</t>
+  </si>
+  <si>
+    <t>Uyga qaytish</t>
+  </si>
+  <si>
+    <t>Kvitansiya yoki pdf skrinshotini joylashtiring</t>
+  </si>
+  <si>
+    <t>Siz noto‘g‘ri fayl yubordingiz, iltimos kvitansiyaning skrinshotini yoki pdf faylini yuboring</t>
+  </si>
+  <si>
+    <t>Sizning faylingiz pdf formatida emas. Kvitansiyaning skrinshotini yoki pdf faylini yuboring</t>
+  </si>
+  <si>
+    <t>Xaridingiz uchun rahmat, administrator tez orada so'rovingizni qabul qiladi</t>
+  </si>
+  <si>
+    <t>Mahsulotni tanlang</t>
+  </si>
+  <si>
+    <t>Stokda mahsulotlar yo'q</t>
+  </si>
+  <si>
+    <t>Avtorizatsiya uchun telefon raqamingizni ulashing</t>
+  </si>
+  <si>
+    <t>Ism</t>
+  </si>
+  <si>
+    <t>Tavsif</t>
+  </si>
+  <si>
+    <t>Narxi</t>
+  </si>
+  <si>
+    <t>Sizning buyurtmangiz</t>
+  </si>
+  <si>
+    <t>Jami</t>
+  </si>
+  <si>
+    <t>Toʻlash uchun &lt;a href = "https://www.google.kz/?hl=ru"&gt;havolaga&lt;/a&gt; oʻting va toʻlang.</t>
+  </si>
+  <si>
+    <t>Quyidagi “Kvitansiyani biriktirish” tugmasini bosish orqali toʻlov kvitansiyasini ilova qiling (kvitansiyaning skrinshoti yoki pdf)</t>
+  </si>
+  <si>
+    <t>Telefonni ulashing</t>
+  </si>
+  <si>
+    <t>Katalog</t>
+  </si>
+  <si>
+    <t>Savat</t>
+  </si>
+  <si>
+    <t>TSS</t>
+  </si>
+  <si>
+    <t>Kontaktlar</t>
+  </si>
+  <si>
+    <t>Tilni o'zgartirish</t>
+  </si>
+  <si>
+    <t>Orqaga</t>
+  </si>
+  <si>
+    <t>Sotib olish</t>
+  </si>
+  <si>
+    <t>Chiqindini bo'shatish</t>
+  </si>
+  <si>
+    <t>Yangi buyurtma!</t>
+  </si>
+  <si>
+    <t>Mobil telefon</t>
+  </si>
+  <si>
+    <t>Buyurtma</t>
+  </si>
+  <si>
+    <t>Siz tilingizni o'zgartirdingiz</t>
+  </si>
+  <si>
+    <t>Ederra Lab 01 Sulfatsiz shampun 600 ml</t>
+  </si>
+  <si>
+    <t>Ederra Lab 01 shampun 600 ml</t>
+  </si>
+  <si>
+    <t>Ederra Lab 03 konditsioner spreyi 200 ml</t>
+  </si>
+  <si>
+    <t>Ederra Lab 02 Intense Moisture Mask niqobi 600 ml</t>
+  </si>
+  <si>
+    <t>Ederra Lab 01 Sulfatsiz shampun 300 ml</t>
+  </si>
+  <si>
+    <t>Ederra Lab 01 shampun 300 ml</t>
+  </si>
+  <si>
+    <t>porlash, namlash, oziqlantirish, mustahkamlash, elastiklik berish, tiklash, tozalash, himoya qilish</t>
+  </si>
+  <si>
+    <t>namlash, oziqlantirish, silliqlash, mustahkamlash, elastiklik berish, antistatik ta'sir, bo'lingan uchlardan himoya qilish, tiklash</t>
+  </si>
+  <si>
+    <t>Bizning kompaniya do'konimizga xush kelibsiz
+Mahsulotlarni tanlash uchun quyidagi asosiy menyudagi Katalogga o'ting</t>
+  </si>
+  <si>
+    <t>Добро пожаловать в магазин нашей компании
+Для выбора продукции перейдите в Каталог в главном меню ниже</t>
+  </si>
+  <si>
+    <t>A, B, E, F, D vitaminlari majmuasini, choy daraxti barglarining faol moddasi va gidrolizlangan kollagenning yuqori konsentratsiyasini o'z ichiga oladi. Sochni molekulyar darajada tiklaydi. Soch va bosh terisini oziqlantiradi va mustahkamlaydi, namlaydi, yog'ni tartibga soluvchi ta'sirga ega. Sochga yumshoqlik, elastiklik, tabiiy porlash va elastiklik beradi.</t>
+  </si>
+  <si>
+    <t>Maxsus konsentrlangan formula choy daraxti barglarining tabiiy bazasidan tayyorlanadi. A, B, E, F, D vitaminlari majmuasi, kollagen va aloe Barbadensis barglari ekstrakti mavjud.</t>
+  </si>
+  <si>
+    <t>Maxsus konsentrlangan formula choy daraxti barglarining tabiiy bazasidan tayyorlanadi. Soch va bosh terisini samarali va muloyimlik bilan tozalaydi, ortiqcha quritishni oldini oladi.</t>
+  </si>
+  <si>
+    <t>rus</t>
+  </si>
+  <si>
+    <t>Русский</t>
+  </si>
+  <si>
+    <t>Узбекский</t>
+  </si>
+  <si>
+    <t>o'zbek</t>
+  </si>
+  <si>
+    <t>- Sulfat shampun: soch va bosh terisidan ortiqcha yog ' va kirni samarali tozalaydi va olib tashlaydi. Chuqur tozalash va tazelik tuyg'usini izlayotganlar uchun mos bo'lishi mumkin. Bundan tashqari, u ko'proq ko'pikka ega.
+- Sulfatsiz shampun: sochlarning tabiiy yog'larini saqlab, yumshoqroq tozalaydi. Tez-tez foydalanish uchun, ayniqsa sezgir bosh terisi va qayta ishlangan sochlar uchun javob beradi.
+Ushbu shampunlarni tanlash tozalik hissi va soch turiga nisbatan shaxsiy xohishingizga bog'liq.</t>
+  </si>
+  <si>
+    <t>03 спрей после использования обогащает волосы аминокислотами и белком, микроколлагеном, делая кортикальный слой волос более прочным, эластичным и здоровым.
+Среди  ингредиентов в составе имеется амодиметикон. Он образовывает на волосах защитную пленку, предотвращающую повреждение волос от высоких температур при укладке. Таким образом, служит компонентом, обеспечивающим определенный уровень термозащиты.</t>
+  </si>
+  <si>
+    <t>03 foydalanishdan keyin buzadigan amallar sochlarni aminokislotalar va oqsil, mikrokollagen bilan boyitadi, bu esa sochlarning kortikal qatlamini yanada mustahkam, elastik va sog'lom qiladi.
+Tarkibdagi ingredientlar orasida amodimetikon mavjud. U sochlarga himoya plyonka hosil qiladi, bu esa soch turmagi paytida yuqori haroratdan sochlarning shikastlanishiga yo'l qo'ymaydi. Shunday qilib, u ma'lum darajada termal himoyani ta'minlaydigan komponent bo'lib xizmat qiladi.</t>
+  </si>
+  <si>
+    <t>so'm</t>
+  </si>
+  <si>
+    <t>сум</t>
+  </si>
+  <si>
+    <t>Spray konditsioner (03), u qanday yordam beradi?</t>
+  </si>
+  <si>
+    <t>Sulfatli va sulfatsiz shampunlar o'rtasidagi farq</t>
+  </si>
+  <si>
+    <t>Сотрудничество</t>
+  </si>
+  <si>
+    <t>Hamkorlik</t>
+  </si>
+  <si>
+    <t>- Шампунь с сульфатом: Эффективно очищает и удаляет излишки масла и грязи с волос и кожи головы. Может подойти для тех, кто ищет глубокое очищение и чувство свежести. Также у него больше пенообразования.
+- Шампунь без сульфата: Более мягко очищает, сохраняя естественные масла волос. Подходит для частого использования, особенно для чувствительной кожи головы и обработанных волос.
+Выбор между этими шампунями зависит от Ваших личных предпочтений в плане ощущения чистоты и типа волос.</t>
+  </si>
+  <si>
+    <t>Разница шампуня с сульфатом и без</t>
+  </si>
+  <si>
+    <t>Как помогает спрей кондиционер</t>
+  </si>
+  <si>
+    <t>По поводу сотрудничества:
+Заполните анкету так и отправьте одним сообщением:
+&lt;i&gt;Имя представителя&lt;/i&gt;
+&lt;i&gt;Должность&lt;/i&gt;
+&lt;i&gt;Город&lt;/i&gt;
+&lt;i&gt;Соц.сети&lt;/i&gt;
+&lt;i&gt;Сайт&lt;/i&gt;
+&lt;i&gt;Телефон&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Hamkorlik haqida:
+Shaklni to'ldiring va uni bitta xabarda yuboring:
+&lt;i&gt;Vakil nomi&lt;/i&gt;
+&lt;i&gt;Pozitsiya&lt;/i&gt;
+&lt;i&gt;Shahar&lt;/i&gt;
+&lt;i&gt;Ijtimoiy tarmoqlar&lt;/i&gt;
+&lt;i&gt;Veb-sayt&lt;/i&gt;
+&lt;i&gt;Telefon&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Подтвердите пожалуйста!</t>
+  </si>
+  <si>
+    <t>Вы написали:</t>
+  </si>
+  <si>
+    <t>Tasdiqlang Iltimos!</t>
+  </si>
+  <si>
+    <t>Siz yozgansiz:</t>
+  </si>
+  <si>
+    <t>Спасибо за обращение, мы скоро с вами свяжемся</t>
+  </si>
+  <si>
+    <t>Biz bilan bog'langaningiz uchun tashakkur, tez orada siz bilan bog'lanamiz</t>
+  </si>
+  <si>
+    <t>Да</t>
+  </si>
+  <si>
+    <t>Изменить текст</t>
+  </si>
+  <si>
+    <t>Ha</t>
+  </si>
+  <si>
+    <t>Matnni o'zgartirish</t>
+  </si>
+  <si>
+    <t>Пришло новое обращение по сотрудничеству!</t>
+  </si>
+  <si>
+    <t>Hamkorlik uchun yangi so'rov keldi!</t>
   </si>
 </sst>
 </file>
@@ -210,10 +463,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -424,15 +685,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="102.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="101.7109375" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -448,250 +709,520 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B12" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B17" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B18" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B19" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B20" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B21" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B22" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B23" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B24" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B25" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B26" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B27" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B28" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B29" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B30" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B31" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B32" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B33" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B34" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B35" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B36" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B37" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B38" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B39" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B40" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B41" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B42" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B43" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B44" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B45" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" ht="15.75" customHeight="1">
+      <c r="B46" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="15.75" customHeight="1">
+        <v>44</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="15.75" customHeight="1">
+        <v>45</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="15.75" customHeight="1">
+        <v>46</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A51" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A51" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A53" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A54" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A55" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A56" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A57" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A58" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A59" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A60" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A61" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A62" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A63" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A64" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A65" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A66" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>